<commit_message>
added JS greedy error
</commit_message>
<xml_diff>
--- a/JSChart.xlsx
+++ b/JSChart.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="JSOutput" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1307,6 +1307,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1351,7 +1407,7 @@
       <c:valAx>
         <c:axId val="327694256"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="30"/>
           <c:orientation val="minMax"/>
           <c:min val="1000"/>
         </c:scaling>
@@ -1371,6 +1427,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t> Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1411,6 +1523,7 @@
         <c:crossAx val="329606792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:minorUnit val="10"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2059,7 +2172,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8673353" cy="6297706"/>
+    <xdr:ext cx="8667750" cy="6296025"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>

</xml_diff>